<commit_message>
Read me for help and excel changes
</commit_message>
<xml_diff>
--- a/Dash.xlsx
+++ b/Dash.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DashApp\DashboardApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1DB0FA83-F5E4-4E23-8042-63B525D1B0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A1353B-6CF7-43CA-9E54-AA98446ECDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{CC886C5E-A2E8-43A6-A757-361F61568B91}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CC886C5E-A2E8-43A6-A757-361F61568B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Dash_1" sheetId="1" r:id="rId1"/>
     <sheet name="Traffic" sheetId="2" r:id="rId2"/>
     <sheet name="Exhibition" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="139">
   <si>
     <t>Date</t>
   </si>
@@ -937,12 +937,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1298,11 +1297,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB81526-73D0-415E-A43A-7B410396AD9C}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1520,1437 +1519,6 @@
       </c>
       <c r="Q4">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>45600</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>129</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>99</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1331.95</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>45601</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>137</v>
-      </c>
-      <c r="D6">
-        <v>37</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1631.83</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>45602</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>136</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-      <c r="E7">
-        <v>103</v>
-      </c>
-      <c r="F7">
-        <v>16474.29</v>
-      </c>
-      <c r="G7">
-        <v>17298</v>
-      </c>
-      <c r="H7">
-        <v>1568.87</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>17298</v>
-      </c>
-      <c r="K7">
-        <v>2</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>8649</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>45603</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>151</v>
-      </c>
-      <c r="D8">
-        <v>52</v>
-      </c>
-      <c r="E8">
-        <v>99</v>
-      </c>
-      <c r="F8">
-        <v>28926.91</v>
-      </c>
-      <c r="G8">
-        <v>30373.25</v>
-      </c>
-      <c r="H8">
-        <v>1559.18</v>
-      </c>
-      <c r="I8">
-        <v>20999</v>
-      </c>
-      <c r="J8">
-        <v>9374.25</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-      <c r="L8">
-        <v>13.47</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>15186.625</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>45604</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>136</v>
-      </c>
-      <c r="D9">
-        <v>31</v>
-      </c>
-      <c r="E9">
-        <v>105</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1471.79</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>45605</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>117</v>
-      </c>
-      <c r="D10">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>102</v>
-      </c>
-      <c r="F10">
-        <v>14092.38</v>
-      </c>
-      <c r="G10">
-        <v>14797</v>
-      </c>
-      <c r="H10">
-        <v>1023.29</v>
-      </c>
-      <c r="I10">
-        <v>10998</v>
-      </c>
-      <c r="J10">
-        <v>3799</v>
-      </c>
-      <c r="K10">
-        <v>3</v>
-      </c>
-      <c r="L10">
-        <v>10.75</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.74</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>4932.3333329999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>45606</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>165</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>140</v>
-      </c>
-      <c r="F11">
-        <v>12380</v>
-      </c>
-      <c r="G11">
-        <v>12999</v>
-      </c>
-      <c r="H11">
-        <v>1614.58</v>
-      </c>
-      <c r="I11">
-        <v>12999</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>12999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>45607</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>267</v>
-      </c>
-      <c r="D12">
-        <v>48</v>
-      </c>
-      <c r="E12">
-        <v>219</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>1940.21</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>45608</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>387</v>
-      </c>
-      <c r="D13">
-        <v>43</v>
-      </c>
-      <c r="E13">
-        <v>344</v>
-      </c>
-      <c r="F13">
-        <v>11903.81</v>
-      </c>
-      <c r="G13">
-        <v>12499</v>
-      </c>
-      <c r="H13">
-        <v>1351.12</v>
-      </c>
-      <c r="I13">
-        <v>12499</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>9.25</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>12499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>45609</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>273</v>
-      </c>
-      <c r="D14">
-        <v>38</v>
-      </c>
-      <c r="E14">
-        <v>235</v>
-      </c>
-      <c r="F14">
-        <v>42378.1</v>
-      </c>
-      <c r="G14">
-        <v>44497</v>
-      </c>
-      <c r="H14">
-        <v>1416.83</v>
-      </c>
-      <c r="I14">
-        <v>12999</v>
-      </c>
-      <c r="J14">
-        <v>31498</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
-      <c r="L14">
-        <v>9.17</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0.71</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>22248.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>45610</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>224</v>
-      </c>
-      <c r="D15">
-        <v>45</v>
-      </c>
-      <c r="E15">
-        <v>179</v>
-      </c>
-      <c r="F15">
-        <v>10951.43</v>
-      </c>
-      <c r="G15">
-        <v>11499</v>
-      </c>
-      <c r="H15">
-        <v>1870.41</v>
-      </c>
-      <c r="I15">
-        <v>11499</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>6.15</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>11499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>45611</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16">
-        <v>157</v>
-      </c>
-      <c r="D16">
-        <v>30</v>
-      </c>
-      <c r="E16">
-        <v>127</v>
-      </c>
-      <c r="F16">
-        <v>16188.58</v>
-      </c>
-      <c r="G16">
-        <v>16998</v>
-      </c>
-      <c r="H16">
-        <v>1519.72</v>
-      </c>
-      <c r="I16">
-        <v>8499</v>
-      </c>
-      <c r="J16">
-        <v>8499</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>5.59</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>8499</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>45612</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>188</v>
-      </c>
-      <c r="D17">
-        <v>35</v>
-      </c>
-      <c r="E17">
-        <v>153</v>
-      </c>
-      <c r="F17">
-        <v>10951.43</v>
-      </c>
-      <c r="G17">
-        <v>11499</v>
-      </c>
-      <c r="H17">
-        <v>1805.82</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>11499</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
-        <v>1</v>
-      </c>
-      <c r="N17" s="2">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>11499</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>45613</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18">
-        <v>253</v>
-      </c>
-      <c r="D18">
-        <v>39</v>
-      </c>
-      <c r="E18">
-        <v>214</v>
-      </c>
-      <c r="F18">
-        <v>13901.91</v>
-      </c>
-      <c r="G18">
-        <v>14597</v>
-      </c>
-      <c r="H18">
-        <v>3325.82</v>
-      </c>
-      <c r="I18">
-        <v>14597</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-      <c r="L18">
-        <v>4.3899999999999997</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>4865.6666670000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>45614</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>745</v>
-      </c>
-      <c r="D19">
-        <v>63</v>
-      </c>
-      <c r="E19">
-        <v>682</v>
-      </c>
-      <c r="F19">
-        <v>22855.24</v>
-      </c>
-      <c r="G19">
-        <v>23998</v>
-      </c>
-      <c r="H19">
-        <v>2377.96</v>
-      </c>
-      <c r="I19">
-        <v>10499</v>
-      </c>
-      <c r="J19">
-        <v>13499</v>
-      </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <v>4.42</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
-        <v>11999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <v>354</v>
-      </c>
-      <c r="D20">
-        <v>58</v>
-      </c>
-      <c r="E20">
-        <v>296</v>
-      </c>
-      <c r="F20">
-        <v>18398.05</v>
-      </c>
-      <c r="G20">
-        <v>19597</v>
-      </c>
-      <c r="H20">
-        <v>2202.89</v>
-      </c>
-      <c r="I20">
-        <v>11999</v>
-      </c>
-      <c r="J20">
-        <v>7598</v>
-      </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
-      <c r="L20">
-        <v>5.45</v>
-      </c>
-      <c r="M20" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="N20" s="2">
-        <v>0.61</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>9798.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>404</v>
-      </c>
-      <c r="D21">
-        <v>46</v>
-      </c>
-      <c r="E21">
-        <v>358</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>480.77</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>45617</v>
-      </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22">
-        <v>224</v>
-      </c>
-      <c r="D22">
-        <v>45</v>
-      </c>
-      <c r="E22">
-        <v>179</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>3046.54</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0</v>
-      </c>
-      <c r="N22" s="2">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>45618</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23">
-        <v>195</v>
-      </c>
-      <c r="D23">
-        <v>45</v>
-      </c>
-      <c r="E23">
-        <v>150</v>
-      </c>
-      <c r="F23">
-        <v>33331.43</v>
-      </c>
-      <c r="G23">
-        <v>34998</v>
-      </c>
-      <c r="H23">
-        <v>3469.46</v>
-      </c>
-      <c r="I23">
-        <v>34998</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>2</v>
-      </c>
-      <c r="L23">
-        <v>10.09</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>17499</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>45619</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24">
-        <v>539</v>
-      </c>
-      <c r="D24">
-        <v>56</v>
-      </c>
-      <c r="E24">
-        <v>483</v>
-      </c>
-      <c r="F24">
-        <v>12380</v>
-      </c>
-      <c r="G24">
-        <v>12999</v>
-      </c>
-      <c r="H24">
-        <v>1167.3599999999999</v>
-      </c>
-      <c r="I24">
-        <v>12999</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>11.14</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0</v>
-      </c>
-      <c r="N24" s="2">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>12999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>45620</v>
-      </c>
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25">
-        <v>548</v>
-      </c>
-      <c r="D25">
-        <v>45</v>
-      </c>
-      <c r="E25">
-        <v>503</v>
-      </c>
-      <c r="F25">
-        <v>6510.7</v>
-      </c>
-      <c r="G25">
-        <v>6999</v>
-      </c>
-      <c r="H25">
-        <v>789.04</v>
-      </c>
-      <c r="I25">
-        <v>6999</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>8.8699999999999992</v>
-      </c>
-      <c r="M25" s="2">
-        <v>0</v>
-      </c>
-      <c r="N25" s="2">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>6999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>45621</v>
-      </c>
-      <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26">
-        <v>446</v>
-      </c>
-      <c r="D26">
-        <v>70</v>
-      </c>
-      <c r="E26">
-        <v>376</v>
-      </c>
-      <c r="F26">
-        <v>9521.9</v>
-      </c>
-      <c r="G26">
-        <v>9521.9</v>
-      </c>
-      <c r="H26">
-        <v>3445.36</v>
-      </c>
-      <c r="I26">
-        <v>5499</v>
-      </c>
-      <c r="J26">
-        <v>4022.9</v>
-      </c>
-      <c r="K26">
-        <v>2</v>
-      </c>
-      <c r="L26">
-        <v>1.6</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="N26" s="2">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>4760.95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>45622</v>
-      </c>
-      <c r="B27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27">
-        <v>339</v>
-      </c>
-      <c r="D27">
-        <v>56</v>
-      </c>
-      <c r="E27">
-        <v>283</v>
-      </c>
-      <c r="F27">
-        <v>10760</v>
-      </c>
-      <c r="G27">
-        <v>23140</v>
-      </c>
-      <c r="H27">
-        <v>3376.79</v>
-      </c>
-      <c r="I27">
-        <v>11298</v>
-      </c>
-      <c r="J27">
-        <v>11842</v>
-      </c>
-      <c r="K27">
-        <v>3</v>
-      </c>
-      <c r="L27">
-        <v>3.35</v>
-      </c>
-      <c r="M27" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="N27" s="2">
-        <v>0.49</v>
-      </c>
-      <c r="O27">
-        <v>3</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>7713.3333329999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>45623</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28">
-        <v>310</v>
-      </c>
-      <c r="D28">
-        <v>52</v>
-      </c>
-      <c r="E28">
-        <v>258</v>
-      </c>
-      <c r="F28">
-        <v>25073</v>
-      </c>
-      <c r="G28">
-        <v>25073</v>
-      </c>
-      <c r="H28">
-        <v>1652.43</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>25073</v>
-      </c>
-      <c r="K28">
-        <v>2</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28" s="2">
-        <v>1</v>
-      </c>
-      <c r="N28" s="2">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>1</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
-        <v>12536.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>45624</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29">
-        <v>390</v>
-      </c>
-      <c r="D29">
-        <v>57</v>
-      </c>
-      <c r="E29">
-        <v>315</v>
-      </c>
-      <c r="F29">
-        <v>27337</v>
-      </c>
-      <c r="G29">
-        <v>27337</v>
-      </c>
-      <c r="H29">
-        <v>2994.88</v>
-      </c>
-      <c r="I29">
-        <v>27337</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>3</v>
-      </c>
-      <c r="L29">
-        <v>18.3</v>
-      </c>
-      <c r="M29" s="2">
-        <v>0</v>
-      </c>
-      <c r="N29" s="2">
-        <v>1</v>
-      </c>
-      <c r="O29">
-        <v>2</v>
-      </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29">
-        <v>9112.3333330000005</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>45625</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30">
-        <v>374</v>
-      </c>
-      <c r="D30">
-        <v>72</v>
-      </c>
-      <c r="E30">
-        <v>301</v>
-      </c>
-      <c r="F30">
-        <v>3618.25</v>
-      </c>
-      <c r="G30">
-        <v>3618.25</v>
-      </c>
-      <c r="H30">
-        <v>2411.9499999999998</v>
-      </c>
-      <c r="I30">
-        <v>3618</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>3</v>
-      </c>
-      <c r="M30" s="2">
-        <v>0</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30">
-        <v>1</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>3618.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>45626</v>
-      </c>
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31">
-        <v>286</v>
-      </c>
-      <c r="D31">
-        <v>52</v>
-      </c>
-      <c r="E31">
-        <v>230</v>
-      </c>
-      <c r="F31">
-        <v>14760</v>
-      </c>
-      <c r="G31">
-        <v>14760</v>
-      </c>
-      <c r="H31">
-        <v>1378.37</v>
-      </c>
-      <c r="I31">
-        <v>14760</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>2</v>
-      </c>
-      <c r="L31">
-        <v>10.7</v>
-      </c>
-      <c r="M31" s="2">
-        <v>0</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31">
-        <v>2</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>7380</v>
       </c>
     </row>
   </sheetData>
@@ -4584,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7A7A2A-5AC6-4291-A7DC-0891D0B37DD4}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
@@ -4620,7 +3188,7 @@
       <c r="H1" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>